<commit_message>
feat: enhance TextEditor component with new toolbar features and remove unused assets
</commit_message>
<xml_diff>
--- a/frontend/src/assets/vocapedia_compose_template.xlsx
+++ b/frontend/src/assets/vocapedia_compose_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="11850"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Yeni XLSX Worksheet" sheetId="1" r:id="rId1"/>
@@ -923,7 +923,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -969,9 +969,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -987,15 +984,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1004,9 +992,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1559,7 +1544,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E15"/>
+      <selection activeCell="K1" sqref="K1:T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15"/>
@@ -1582,19 +1567,19 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="30"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="3"/>
@@ -1606,17 +1591,17 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="31"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="26"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="5"/>
@@ -1628,17 +1613,17 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="31"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="26"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="7" t="s">
@@ -1652,17 +1637,17 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="31"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="26"/>
     </row>
     <row r="5" ht="15.75" spans="1:20">
       <c r="A5" s="9" t="s">
@@ -1678,17 +1663,17 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="31"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="26"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="13" t="s">
@@ -1707,20 +1692,20 @@
       <c r="H6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="31"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="26"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="13"/>
@@ -1737,20 +1722,20 @@
       <c r="H7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="31"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="26"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="13" t="s">
@@ -1769,20 +1754,20 @@
       <c r="H8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="31"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="26"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="13"/>
@@ -1799,20 +1784,20 @@
       <c r="H9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="31"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="26"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="13" t="s">
@@ -1831,20 +1816,20 @@
       <c r="H10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="31"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="26"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="13"/>
@@ -1861,20 +1846,20 @@
       <c r="H11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="31"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="26"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="13" t="s">
@@ -1893,20 +1878,20 @@
       <c r="H12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="24"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="31"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="26"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="13"/>
@@ -1923,20 +1908,20 @@
       <c r="H13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="31"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="26"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="13" t="s">
@@ -1955,20 +1940,20 @@
       <c r="H14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="31"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="26"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="13"/>
@@ -1985,20 +1970,20 @@
       <c r="H15" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="31"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="26"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="13" t="s">
@@ -2017,20 +2002,20 @@
       <c r="H16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="31"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="26"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="13"/>
@@ -2047,20 +2032,20 @@
       <c r="H17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="31"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="26"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="13" t="s">
@@ -2079,20 +2064,20 @@
       <c r="H18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="24"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="31"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="26"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="13"/>
@@ -2109,20 +2094,20 @@
       <c r="H19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="31"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="26"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="13" t="s">
@@ -2141,20 +2126,20 @@
       <c r="H20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="31"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="26"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="13"/>
@@ -2171,22 +2156,22 @@
       <c r="H21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="31"/>
-    </row>
-    <row r="22" ht="15.75" spans="1:20">
+      <c r="J21" s="20"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="26"/>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" s="13" t="s">
         <v>5</v>
       </c>
@@ -2203,22 +2188,22 @@
       <c r="H22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="31"/>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="J22" s="20"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="26"/>
+    </row>
+    <row r="23" ht="15.75" spans="1:20">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -2233,60 +2218,60 @@
       <c r="H23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="24" t="s">
+      <c r="I23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="32"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="27"/>
     </row>
     <row r="24" spans="11:20">
-      <c r="K24" s="27" t="s">
+      <c r="K24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
     </row>
     <row r="25" spans="11:20">
-      <c r="K25" s="27" t="s">
+      <c r="K25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
     </row>
     <row r="26" spans="11:20">
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="29"/>
-      <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="34">

</xml_diff>